<commit_message>
Added image pading and teeth locations adjustment
</commit_message>
<xml_diff>
--- a/data-1.xlsx
+++ b/data-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwoodson\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACF0A20F-F3C8-44DE-AE42-852166D55EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D501F68-1B5B-471D-88E3-B44B9CEA7F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29352" yWindow="1560" windowWidth="21324" windowHeight="13428" xr2:uid="{CA13E8D8-0FA6-4F69-B072-6C5B6D41D2A1}"/>
+    <workbookView xWindow="7428" yWindow="1416" windowWidth="21336" windowHeight="13428" xr2:uid="{CA13E8D8-0FA6-4F69-B072-6C5B6D41D2A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,53 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>1-7</t>
+  </si>
+  <si>
+    <t>1-6</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>2-1</t>
+  </si>
+  <si>
+    <t>2-2</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2-4</t>
+  </si>
+  <si>
+    <t>2-5</t>
+  </si>
+  <si>
+    <t>2-6</t>
+  </si>
+  <si>
+    <t>2-7</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -113,13 +160,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,583 +482,627 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972911D0-4D27-42AD-8E7D-4DFC65FD841D}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>-2.7141317103618752</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B2" s="1">
         <v>4.2669910441767449</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C2" s="1">
         <v>0.69920472708358405</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D2" s="1">
         <v>0.34972973417635123</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E2" s="1">
         <v>0.21415665308468848</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F2" s="1">
         <v>-0.10272353208237942</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G2" s="1">
         <v>8.2895620093395184E-2</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H2" s="1">
         <v>9.4144432669603297</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I2" s="1">
         <v>1.00336512496962</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J2" s="1">
         <v>2.7288559265184587</v>
       </c>
-      <c r="K1" s="1">
+      <c r="K2" s="1">
         <v>-1.6238027634841017</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L2" s="1">
         <v>-1.5947008171729089</v>
       </c>
-      <c r="M1" s="1">
+      <c r="M2" s="1">
         <v>-1.8989500137727631</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N2" s="2">
         <v>0.81103580197543745</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>-2.4520584275474588</v>
-      </c>
-      <c r="B2">
-        <v>4.4040041052373633</v>
-      </c>
-      <c r="C2">
-        <v>0.7078001810642961</v>
-      </c>
-      <c r="D2">
-        <v>-5.1969158866535733E-2</v>
-      </c>
-      <c r="E2">
-        <v>-7.6618022257223042E-2</v>
-      </c>
-      <c r="F2">
-        <v>0.26696778513669861</v>
-      </c>
-      <c r="G2">
-        <v>2.0271442862082587</v>
-      </c>
-      <c r="H2">
-        <v>7.6325921506692387</v>
-      </c>
-      <c r="I2">
-        <v>0.87420364046110366</v>
-      </c>
-      <c r="J2">
-        <v>3.2374264995000033</v>
-      </c>
-      <c r="K2">
-        <v>-1.8451238154043177</v>
-      </c>
-      <c r="L2">
-        <v>-1.3121335510614558</v>
-      </c>
-      <c r="M2">
-        <v>-1.8763532091194179</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0.99710385996525019</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>-2.2476812542998501</v>
+        <v>-2.4520584275474588</v>
       </c>
       <c r="B3">
-        <v>4.5799939228311501</v>
+        <v>4.4040041052373633</v>
       </c>
       <c r="C3">
-        <v>0.45350073313771361</v>
+        <v>0.7078001810642961</v>
       </c>
       <c r="D3">
-        <v>-0.76302051635296697</v>
+        <v>-5.1969158866535733E-2</v>
       </c>
       <c r="E3">
-        <v>0.40494708589850092</v>
+        <v>-7.6618022257223042E-2</v>
       </c>
       <c r="F3">
-        <v>0.51756168991444296</v>
+        <v>0.26696778513669861</v>
       </c>
       <c r="G3">
-        <v>3.3010487976833538</v>
+        <v>2.0271442862082587</v>
       </c>
       <c r="H3">
-        <v>6.7873675192986305</v>
+        <v>7.6325921506692387</v>
       </c>
       <c r="I3">
-        <v>0.90674586829346604</v>
+        <v>0.87420364046110366</v>
       </c>
       <c r="J3">
-        <v>2.9637462361705031</v>
+        <v>3.2374264995000033</v>
       </c>
       <c r="K3">
-        <v>-2.0239378787727715</v>
+        <v>-1.8451238154043177</v>
       </c>
       <c r="L3">
-        <v>-1.0369789926886268</v>
+        <v>-1.3121335510614558</v>
       </c>
       <c r="M3">
-        <v>-1.7474060120595354</v>
+        <v>-1.8763532091194179</v>
       </c>
       <c r="N3" s="3">
-        <v>1.2476445479847258</v>
+        <v>0.99710385996525019</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>-2.0265858788965252</v>
+        <v>-2.2476812542998501</v>
       </c>
       <c r="B4">
-        <v>4.5627648084183905</v>
+        <v>4.5799939228311501</v>
       </c>
       <c r="C4">
-        <v>0.60640314141073337</v>
+        <v>0.45350073313771361</v>
       </c>
       <c r="D4">
-        <v>-1.171553823146398</v>
+        <v>-0.76302051635296697</v>
       </c>
       <c r="E4">
-        <v>0.12126984950757796</v>
+        <v>0.40494708589850092</v>
       </c>
       <c r="F4">
-        <v>0.16255077368710677</v>
+        <v>0.51756168991444296</v>
       </c>
       <c r="G4">
-        <v>6.172425439414905</v>
+        <v>3.3010487976833538</v>
       </c>
       <c r="H4">
-        <v>5.1159230394909994</v>
+        <v>6.7873675192986305</v>
       </c>
       <c r="I4">
-        <v>0.9129968942653448</v>
+        <v>0.90674586829346604</v>
       </c>
       <c r="J4">
-        <v>3.1633758657949937</v>
+        <v>2.9637462361705031</v>
       </c>
       <c r="K4">
-        <v>-2.0905477423669061</v>
+        <v>-2.0239378787727715</v>
       </c>
       <c r="L4">
-        <v>-0.87387777549114209</v>
+        <v>-1.0369789926886268</v>
       </c>
       <c r="M4">
-        <v>-1.7282172861912166</v>
+        <v>-1.7474060120595354</v>
       </c>
       <c r="N4" s="3">
-        <v>1.4206617184462911</v>
+        <v>1.2476445479847258</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>-2.0334997960389165</v>
+        <v>-2.0265858788965252</v>
       </c>
       <c r="B5">
-        <v>4.4943987276727979</v>
+        <v>4.5627648084183905</v>
       </c>
       <c r="C5">
-        <v>0.74952134892576572</v>
+        <v>0.60640314141073337</v>
       </c>
       <c r="D5">
-        <v>-1.5377673818474975</v>
+        <v>-1.171553823146398</v>
       </c>
       <c r="E5">
-        <v>-0.35036051697126702</v>
+        <v>0.12126984950757796</v>
       </c>
       <c r="F5">
-        <v>0.3859742636755748</v>
+        <v>0.16255077368710677</v>
       </c>
       <c r="G5">
-        <v>10.120819563517262</v>
+        <v>6.172425439414905</v>
       </c>
       <c r="H5">
-        <v>2.7760727001275067</v>
+        <v>5.1159230394909994</v>
       </c>
       <c r="I5">
-        <v>0.51105603238620378</v>
+        <v>0.9129968942653448</v>
       </c>
       <c r="J5">
-        <v>3.4935054155575527</v>
+        <v>3.1633758657949937</v>
       </c>
       <c r="K5">
-        <v>-2.3005796017246327</v>
+        <v>-2.0905477423669061</v>
       </c>
       <c r="L5">
-        <v>-0.65936103992426709</v>
+        <v>-0.87387777549114209</v>
       </c>
       <c r="M5">
-        <v>-2.0048042050702812</v>
+        <v>-1.7282172861912166</v>
       </c>
       <c r="N5" s="3">
-        <v>1.5172899080332212</v>
+        <v>1.4206617184462911</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>-1.8050786795674592</v>
+        <v>-2.0334997960389165</v>
       </c>
       <c r="B6">
-        <v>4.1504334867617239</v>
+        <v>4.4943987276727979</v>
       </c>
       <c r="C6">
-        <v>1.1857979610589899</v>
+        <v>0.74952134892576572</v>
       </c>
       <c r="D6">
-        <v>-2.083608386338518</v>
+        <v>-1.5377673818474975</v>
       </c>
       <c r="E6">
-        <v>-0.42844495720964398</v>
+        <v>-0.35036051697126702</v>
       </c>
       <c r="F6">
-        <v>0.44120034381208689</v>
+        <v>0.3859742636755748</v>
       </c>
       <c r="G6">
-        <v>15.750272691615919</v>
+        <v>10.120819563517262</v>
       </c>
       <c r="H6">
-        <v>1.1002682021617702</v>
+        <v>2.7760727001275067</v>
       </c>
       <c r="I6">
-        <v>-0.28585540652181562</v>
+        <v>0.51105603238620378</v>
       </c>
       <c r="J6">
-        <v>3.7277952235845131</v>
+        <v>3.4935054155575527</v>
       </c>
       <c r="K6">
-        <v>-2.1932931613468098</v>
+        <v>-2.3005796017246327</v>
       </c>
       <c r="L6">
-        <v>-0.32929833777916978</v>
+        <v>-0.65936103992426709</v>
       </c>
       <c r="M6">
-        <v>-2.1157332361475323</v>
+        <v>-2.0048042050702812</v>
       </c>
       <c r="N6" s="3">
-        <v>1.5910523198165356</v>
+        <v>1.5172899080332212</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>-1.4993076816222477</v>
+        <v>-1.8050786795674592</v>
       </c>
       <c r="B7">
-        <v>4.344273054332298</v>
+        <v>4.1504334867617239</v>
       </c>
       <c r="C7">
-        <v>1.6707884968192281</v>
+        <v>1.1857979610589899</v>
       </c>
       <c r="D7">
-        <v>-2.776889785409657</v>
+        <v>-2.083608386338518</v>
       </c>
       <c r="E7">
-        <v>-0.46746420427721252</v>
+        <v>-0.42844495720964398</v>
       </c>
       <c r="F7">
-        <v>0.50583198480048597</v>
+        <v>0.44120034381208689</v>
       </c>
       <c r="G7">
-        <v>22.06549615983797</v>
+        <v>15.750272691615919</v>
       </c>
       <c r="H7">
-        <v>8.3893888423995935E-2</v>
+        <v>1.1002682021617702</v>
       </c>
       <c r="I7">
-        <v>-1.8006061926863077</v>
+        <v>-0.28585540652181562</v>
       </c>
       <c r="J7">
-        <v>4.0814776291262049</v>
+        <v>3.7277952235845131</v>
       </c>
       <c r="K7">
-        <v>-2.2224691599928632</v>
+        <v>-2.1932931613468098</v>
       </c>
       <c r="L7">
-        <v>-0.25364253007263299</v>
+        <v>-0.32929833777916978</v>
       </c>
       <c r="M7">
-        <v>-1.8679103234176353</v>
+        <v>-2.1157332361475323</v>
       </c>
       <c r="N7" s="3">
-        <v>1.9187169032929441</v>
+        <v>1.5910523198165356</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>-2.3536293904256098</v>
+        <v>-1.4993076816222477</v>
       </c>
       <c r="B8">
-        <v>4.2091155178667243</v>
+        <v>4.344273054332298</v>
       </c>
       <c r="C8">
-        <v>1.1008984439966505</v>
+        <v>1.6707884968192281</v>
       </c>
       <c r="D8">
-        <v>-2.582503137413072</v>
+        <v>-2.776889785409657</v>
       </c>
       <c r="E8">
-        <v>0.93404502822939872</v>
+        <v>-0.46746420427721252</v>
       </c>
       <c r="F8">
-        <v>0.17585625820090814</v>
+        <v>0.50583198480048597</v>
       </c>
       <c r="G8">
-        <v>11.035745123933891</v>
+        <v>22.06549615983797</v>
       </c>
       <c r="H8">
-        <v>4.9933714281081496</v>
+        <v>8.3893888423995935E-2</v>
       </c>
       <c r="I8">
-        <v>-0.78823973441431006</v>
+        <v>-1.8006061926863077</v>
       </c>
       <c r="J8">
-        <v>3.2946566872717131</v>
+        <v>4.0814776291262049</v>
       </c>
       <c r="K8">
-        <v>-2.444613192354125</v>
+        <v>-2.2224691599928632</v>
       </c>
       <c r="L8">
-        <v>-0.9028551103415593</v>
+        <v>-0.25364253007263299</v>
       </c>
       <c r="M8">
-        <v>-2.0209934680915218</v>
+        <v>-1.8679103234176353</v>
       </c>
       <c r="N8" s="3">
-        <v>1.6330707695654911</v>
+        <v>1.9187169032929441</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>-2.6381259801348267</v>
+        <v>-2.3536293904256098</v>
       </c>
       <c r="B9">
-        <v>4.0991875505440873</v>
+        <v>4.2091155178667243</v>
       </c>
       <c r="C9">
-        <v>0.80011331126975693</v>
+        <v>1.1008984439966505</v>
       </c>
       <c r="D9">
-        <v>-2.291383938399115</v>
+        <v>-2.582503137413072</v>
       </c>
       <c r="E9">
-        <v>1.745935039845945</v>
+        <v>0.93404502822939872</v>
       </c>
       <c r="F9">
-        <v>0.17869565290494113</v>
+        <v>0.17585625820090814</v>
       </c>
       <c r="G9">
-        <v>4.8479270194342758</v>
+        <v>11.035745123933891</v>
       </c>
       <c r="H9">
-        <v>8.3437276350209348</v>
+        <v>4.9933714281081496</v>
       </c>
       <c r="I9">
-        <v>-0.16509283886031664</v>
+        <v>-0.78823973441431006</v>
       </c>
       <c r="J9">
-        <v>2.7400390637277581</v>
+        <v>3.2946566872717131</v>
       </c>
       <c r="K9">
-        <v>-2.3137417845907682</v>
+        <v>-2.444613192354125</v>
       </c>
       <c r="L9">
-        <v>-1.1697750508458598</v>
+        <v>-0.9028551103415593</v>
       </c>
       <c r="M9">
-        <v>-2.238918111146841</v>
+        <v>-2.0209934680915218</v>
       </c>
       <c r="N9" s="3">
-        <v>1.2642050335721289</v>
+        <v>1.6330707695654911</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>-2.7668317093926991</v>
+        <v>-2.6381259801348267</v>
       </c>
       <c r="B10">
-        <v>4.0894699692001382</v>
+        <v>4.0991875505440873</v>
       </c>
       <c r="C10">
-        <v>0.62973160036149178</v>
+        <v>0.80011331126975693</v>
       </c>
       <c r="D10">
-        <v>-1.1330474749556152</v>
+        <v>-2.291383938399115</v>
       </c>
       <c r="E10">
-        <v>1.6202737695405696</v>
+        <v>1.745935039845945</v>
       </c>
       <c r="F10">
-        <v>0.26488318990473592</v>
+        <v>0.17869565290494113</v>
       </c>
       <c r="G10">
-        <v>3.092569659670243</v>
+        <v>4.8479270194342758</v>
       </c>
       <c r="H10">
-        <v>9.5959122289668404</v>
+        <v>8.3437276350209348</v>
       </c>
       <c r="I10">
-        <v>0.30224394381329561</v>
+        <v>-0.16509283886031664</v>
       </c>
       <c r="J10">
-        <v>2.4724247652024967</v>
+        <v>2.7400390637277581</v>
       </c>
       <c r="K10">
-        <v>-2.2104100457637572</v>
+        <v>-2.3137417845907682</v>
       </c>
       <c r="L10">
-        <v>-1.1290333260862777</v>
+        <v>-1.1697750508458598</v>
       </c>
       <c r="M10">
-        <v>-2.2602220067151917</v>
+        <v>-2.238918111146841</v>
       </c>
       <c r="N10" s="3">
-        <v>1.1426125720874287</v>
+        <v>1.2642050335721289</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>-3.1366493950716769</v>
+        <v>-2.7668317093926991</v>
       </c>
       <c r="B11">
-        <v>3.7474534268437356</v>
+        <v>4.0894699692001382</v>
       </c>
       <c r="C11">
-        <v>0.62593462820593437</v>
+        <v>0.62973160036149178</v>
       </c>
       <c r="D11">
-        <v>-0.31058778393788755</v>
+        <v>-1.1330474749556152</v>
       </c>
       <c r="E11">
-        <v>0.95110600718754656</v>
+        <v>1.6202737695405696</v>
       </c>
       <c r="F11">
-        <v>0.10273755564586264</v>
+        <v>0.26488318990473592</v>
       </c>
       <c r="G11">
-        <v>1.3202154499785328</v>
+        <v>3.092569659670243</v>
       </c>
       <c r="H11">
-        <v>10.224378321653173</v>
+        <v>9.5959122289668404</v>
       </c>
       <c r="I11">
-        <v>0.46401457994014872</v>
+        <v>0.30224394381329561</v>
       </c>
       <c r="J11">
-        <v>2.982545472034015</v>
+        <v>2.4724247652024967</v>
       </c>
       <c r="K11">
-        <v>-2.0202390128278953</v>
+        <v>-2.2104100457637572</v>
       </c>
       <c r="L11">
-        <v>-1.3611486651307325</v>
+        <v>-1.1290333260862777</v>
       </c>
       <c r="M11">
-        <v>-2.2056005074580627</v>
+        <v>-2.2602220067151917</v>
       </c>
       <c r="N11" s="3">
-        <v>1.1385671869671483</v>
+        <v>1.1426125720874287</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
+        <v>-3.1366493950716769</v>
+      </c>
+      <c r="B12">
+        <v>3.7474534268437356</v>
+      </c>
+      <c r="C12">
+        <v>0.62593462820593437</v>
+      </c>
+      <c r="D12">
+        <v>-0.31058778393788755</v>
+      </c>
+      <c r="E12">
+        <v>0.95110600718754656</v>
+      </c>
+      <c r="F12">
+        <v>0.10273755564586264</v>
+      </c>
+      <c r="G12">
+        <v>1.3202154499785328</v>
+      </c>
+      <c r="H12">
+        <v>10.224378321653173</v>
+      </c>
+      <c r="I12">
+        <v>0.46401457994014872</v>
+      </c>
+      <c r="J12">
+        <v>2.982545472034015</v>
+      </c>
+      <c r="K12">
+        <v>-2.0202390128278953</v>
+      </c>
+      <c r="L12">
+        <v>-1.3611486651307325</v>
+      </c>
+      <c r="M12">
+        <v>-2.2056005074580627</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1.1385671869671483</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>-3.417347245458529</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>3.844527123719891</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>0.59142611221881625</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>0.4662440751193983</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>0.59751804662856789</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>0.10530076692234952</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>-0.21492501171865575</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>10.896372768680589</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>0.66875860151985012</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <v>2.8128290101375524</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>-1.9295286897676847</v>
       </c>
-      <c r="L12">
+      <c r="L13">
         <v>-1.2598698778487083</v>
       </c>
-      <c r="M12">
+      <c r="M13">
         <v>-2.4968351651352707</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N13" s="3">
         <v>0.87364009601898063</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>-3.4817018122905092</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B14" s="4">
         <v>3.8853563884853695</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C14" s="4">
         <v>0.27966479170500419</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D14" s="4">
         <v>0.21402161946675258</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E14" s="4">
         <v>0.36284958943335177</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F14" s="4">
         <v>9.6226984494824461E-2</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G14" s="4">
         <v>-1.5527008874394173</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H14" s="4">
         <v>11.785947451537401</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I14" s="4">
         <v>0.51670859585271489</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J14" s="4">
         <v>3.1554419516167438</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K14" s="4">
         <v>-1.9183408900926424</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L14" s="4">
         <v>-1.1188503987825011</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M14" s="4">
         <v>-2.3284413821983181</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N14" s="5">
         <v>0.91968028616140618</v>
       </c>
     </row>

</xml_diff>